<commit_message>
Realise that v9 still stores all the multiples of 3, & also does the whole auto-expanding-rolling-array thing, so for the tree search idea we really want to be starting from one of the later versions. The extended version so far just worked on incomplete parts of v9 (column 1 is now easily computable, though the results arent used for column 2 so that's broken), so rename the v9-extended to v9 (& update descriptions)
</commit_message>
<xml_diff>
--- a/C++ v9/expReg(1) last pattern positions.xlsx
+++ b/C++ v9/expReg(1) last pattern positions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\_Edu\2019\Semester 1\Random\CollatzThing\CollatzExperiments\C++ v9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\_Edu\2019\Semester 1\Random\CollatzThing\CollatzExperiments\C++ v9-extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+  <si>
+    <t>ok to miss</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>ok to miss as we already check for powers of 2 and overlay a superset of on bits</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,18 +357,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -362,8 +377,11 @@
         <f>SUBSTITUTE(SUBSTITUTE(_xlfn.BASE(A1,2,10), "0", "-"), "1", "#")</f>
         <v>---------#</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -371,8 +389,11 @@
         <f t="shared" ref="B2:B54" si="0">SUBSTITUTE(SUBSTITUTE(_xlfn.BASE(A2,2,10), "0", "-"), "1", "#")</f>
         <v>--------#-</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -380,8 +401,11 @@
         <f t="shared" si="0"/>
         <v>-------#--</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -390,7 +414,7 @@
         <v>-------#-#</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -399,7 +423,7 @@
         <v>-------###</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -407,8 +431,11 @@
         <f t="shared" si="0"/>
         <v>------#---</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -417,7 +444,7 @@
         <v>------#-#-</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -426,7 +453,7 @@
         <v>------#-##</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -435,7 +462,7 @@
         <v>------###-</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16</v>
       </c>
@@ -443,8 +470,11 @@
         <f t="shared" si="0"/>
         <v>-----#----</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>19</v>
       </c>
@@ -453,7 +483,7 @@
         <v>-----#--##</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -462,7 +492,7 @@
         <v>-----#-#--</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>22</v>
       </c>
@@ -471,7 +501,7 @@
         <v>-----#-##-</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>28</v>
       </c>
@@ -480,7 +510,7 @@
         <v>-----###--</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32</v>
       </c>
@@ -488,8 +518,11 @@
         <f t="shared" si="0"/>
         <v>----#-----</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>35</v>
       </c>

</xml_diff>